<commit_message>
Git notes update , added the kgen part and installing WSL details
</commit_message>
<xml_diff>
--- a/SEVEN_Kakfa_Links.xlsx
+++ b/SEVEN_Kakfa_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A233C1F\Documents\Docs&amp;Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA2C45-F8C0-42F8-AE0C-5F1DD3C909A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7249CBF-5088-4B64-A30E-430293728C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21945" yWindow="5055" windowWidth="19515" windowHeight="11610" xr2:uid="{9D751822-9D83-4D60-B2B6-9E7CF2D78AD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>https://rewe.atlassian.net/wiki/spaces/TITISEVEN/pages/1134952479/System+overview+Kafka+Clusters+managed+by+Team+SEVEN</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Comment 1</t>
+  </si>
+  <si>
+    <t>https://grafana.metrics.rewe.cloud/alerting/list</t>
+  </si>
+  <si>
+    <t>Kafka Grafana</t>
   </si>
 </sst>
 </file>
@@ -289,8 +295,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}" name="Table3" displayName="Table3" ref="A3:C11" totalsRowShown="0">
-  <autoFilter ref="A3:C11" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}" name="Table3" displayName="Table3" ref="A3:C12" totalsRowShown="0">
+  <autoFilter ref="A3:C12" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92DEE286-5F23-49AE-A993-EE800877A5EE}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16826D26-E8CF-4027-A8E6-28B0A1A1041D}" name="URL" dataCellStyle="Hyperlink"/>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51094AFD-03E5-4E2E-A855-873D3CEE7610}">
-  <dimension ref="A3:C11"/>
+  <dimension ref="A3:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,6 +714,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{647F7716-5A52-4BF3-9B08-BCC1B789DC54}"/>
@@ -717,11 +731,12 @@
     <hyperlink ref="B9" r:id="rId5" xr:uid="{05DBEA20-3695-490C-93E6-102AAED9E6DE}"/>
     <hyperlink ref="B10" r:id="rId6" xr:uid="{A82AE5B1-B074-4F20-A1EE-F4A97F50477A}"/>
     <hyperlink ref="B11" r:id="rId7" xr:uid="{4233B4E2-FA5D-4231-82C5-0DEBEE98C968}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{F04C5879-D231-445B-930D-ECD231A12A54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates work week Feb 9th 2026
</commit_message>
<xml_diff>
--- a/SEVEN_Kakfa_Links.xlsx
+++ b/SEVEN_Kakfa_Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A233C1F\Documents\Docs&amp;Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7249CBF-5088-4B64-A30E-430293728C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A78DBE-D91B-4568-9054-5F953B4E7069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21945" yWindow="5055" windowWidth="19515" windowHeight="11610" xr2:uid="{9D751822-9D83-4D60-B2B6-9E7CF2D78AD8}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>https://rewe.atlassian.net/wiki/spaces/TITISEVEN/pages/1134952479/System+overview+Kafka+Clusters+managed+by+Team+SEVEN</t>
   </si>
@@ -186,6 +187,12 @@
   </si>
   <si>
     <t>Kafka Grafana</t>
+  </si>
+  <si>
+    <t>https://rewe.atlassian.net/wiki/spaces/O11Y/pages/1211416349/User+Guide+Logscale+Grafana+Loki+Migration</t>
+  </si>
+  <si>
+    <t>Loki</t>
   </si>
 </sst>
 </file>
@@ -295,8 +302,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}" name="Table3" displayName="Table3" ref="A3:C12" totalsRowShown="0">
-  <autoFilter ref="A3:C12" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}" name="Table3" displayName="Table3" ref="A3:C13" totalsRowShown="0">
+  <autoFilter ref="A3:C13" xr:uid="{4FEFBF19-B0BB-4FF9-82D1-B22F0F681040}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92DEE286-5F23-49AE-A993-EE800877A5EE}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16826D26-E8CF-4027-A8E6-28B0A1A1041D}" name="URL" dataCellStyle="Hyperlink"/>
@@ -623,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51094AFD-03E5-4E2E-A855-873D3CEE7610}">
-  <dimension ref="A3:C12"/>
+  <dimension ref="A3:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,6 +729,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{647F7716-5A52-4BF3-9B08-BCC1B789DC54}"/>
@@ -732,11 +747,12 @@
     <hyperlink ref="B10" r:id="rId6" xr:uid="{A82AE5B1-B074-4F20-A1EE-F4A97F50477A}"/>
     <hyperlink ref="B11" r:id="rId7" xr:uid="{4233B4E2-FA5D-4231-82C5-0DEBEE98C968}"/>
     <hyperlink ref="B12" r:id="rId8" xr:uid="{F04C5879-D231-445B-930D-ECD231A12A54}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{5A6AE6C9-548A-4156-8643-080D848DAC3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>